<commit_message>
Added Tool based Code Analysis report and the code improvements
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\anul_3\VVSS\Lab01\CheckLists\CheckLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\faculta\VVSS\lab\Inventory\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE16C6C-5A90-4450-AB59-7527D4A01CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD77093F-F525-44C9-BB2C-F971789AD9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -208,6 +208,93 @@
   </si>
   <si>
     <t>variabila isFound faciliteaza posibilitatea de a returna un produs cand inventarul este vid</t>
+  </si>
+  <si>
+    <t>java:S2095: use try-with-resources for "BufferedReader"</t>
+  </si>
+  <si>
+    <t>Folosim try-with-resources, care se ocupa singur de close si e cod mai readable</t>
+  </si>
+  <si>
+    <t>InventoryRepository / 26, 78, 133</t>
+  </si>
+  <si>
+    <t>Se initializeaza o variabila de tip BufferedReader / BufferedWriter si nu se da close niciodata la acest file descriptor.</t>
+  </si>
+  <si>
+    <t>InventoryRepository / 139</t>
+  </si>
+  <si>
+    <t>java:S1643: Strings should not be concatenated using '+' in a loop</t>
+  </si>
+  <si>
+    <t>Variabila "line" este de tip String si in interiorul unui loop se creeaza din nou o clasa de tip String pentru a-i fi modificata valoarea</t>
+  </si>
+  <si>
+    <t>Folosim un StringBuilder pentru line, si abia dupa ce terminam de construit string-ul prin loop, instantiam variabila de tip String</t>
+  </si>
+  <si>
+    <t>InventoryRepository / 34, 85</t>
+  </si>
+  <si>
+    <t>java:S2147: Catches should be combined</t>
+  </si>
+  <si>
+    <t>Two different catches for 2 different errors that are handled the same way.</t>
+  </si>
+  <si>
+    <t>We combine the two catches into one</t>
+  </si>
+  <si>
+    <t>java:S125: Sections of code should not be commented out</t>
+  </si>
+  <si>
+    <t>InventoryRepository / 22, 69, 117</t>
+  </si>
+  <si>
+    <t>There are lines containing commented out code that make the rest of the code not easily readable.</t>
+  </si>
+  <si>
+    <t>Removed commented out code.</t>
+  </si>
+  <si>
+    <t>Product / 61</t>
+  </si>
+  <si>
+    <t>java:S1656: Variables should not be self-assigned</t>
+  </si>
+  <si>
+    <t>Clasa primeste prin metoda setAssociatedParts o noua valoarea pentru proprietatea cu acelasi nume, dar cine a scris metoda a facut o greseala si asigneaza valoarea primita ca parametru la aceeasi variabila.</t>
+  </si>
+  <si>
+    <t>Valoarea parametrului primit va fi asignata proprietatii associatedParts a clasei Product.</t>
+  </si>
+  <si>
+    <t>Product / 141</t>
+  </si>
+  <si>
+    <t>java:S1155: Collection.isEmpty() should be used to test for emptiness</t>
+  </si>
+  <si>
+    <t>Comparing the size of the collection with 1 to check emptiness.</t>
+  </si>
+  <si>
+    <t>Checking using the method 'isEmpty()'.</t>
+  </si>
+  <si>
+    <t>Product / 11</t>
+  </si>
+  <si>
+    <t>java:S2129: Constructors should not be used to instantiate "String", "BigInteger", "BigDecimal" and primitive-wrap</t>
+  </si>
+  <si>
+    <t>Product / 99</t>
+  </si>
+  <si>
+    <t>There is instantiated a class of type Integer just to call the method 'toString()' on the int variable.</t>
+  </si>
+  <si>
+    <t>Use the static method 'Integer.toString(var)' on the int 'var' instead of instantiating and Integer.</t>
   </si>
 </sst>
 </file>
@@ -422,6 +509,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -464,7 +552,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,19 +882,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -827,10 +914,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -841,10 +928,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -856,15 +943,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -887,7 +974,7 @@
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="21" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1095,19 +1182,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1127,10 +1214,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1141,10 +1228,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1156,15 +1243,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1372,7 +1459,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1393,19 +1480,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1425,10 +1512,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1439,10 +1526,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1454,15 +1541,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1712,18 +1799,18 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="6"/>
@@ -1734,19 +1821,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1766,8 +1853,8 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1778,8 +1865,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1791,8 +1878,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1812,84 +1899,148 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
@@ -2022,11 +2173,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>